<commit_message>
Code Refactoring and API Postman Collections
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Mars.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Mars.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="520" windowWidth="13120" windowHeight="3740" activeTab="1"/>
+    <workbookView xWindow="530" yWindow="520" windowWidth="13120" windowHeight="3740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="SignUp" sheetId="2" r:id="rId2"/>
+    <sheet name="AddSkill" sheetId="3" r:id="rId3"/>
+    <sheet name="UpdateSkill" sheetId="4" r:id="rId4"/>
+    <sheet name="RemoveSkill" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>username</t>
   </si>
@@ -54,12 +57,124 @@
   </si>
   <si>
     <t>Eer</t>
+  </si>
+  <si>
+    <t>Would like to provide selenium training for beginners</t>
+  </si>
+  <si>
+    <t>Programming &amp; Tech</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>One-off service</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Skill-Exchange</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>LocationType</t>
+  </si>
+  <si>
+    <t>Startdate</t>
+  </si>
+  <si>
+    <t>Enddate</t>
+  </si>
+  <si>
+    <t>Selectday</t>
+  </si>
+  <si>
+    <t>Starttime</t>
+  </si>
+  <si>
+    <t>Endtime</t>
+  </si>
+  <si>
+    <t>SkillTrade</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Selenium Web Driver</t>
+  </si>
+  <si>
+    <t>Keen to teach API testing using Postman tool</t>
+  </si>
+  <si>
+    <t>Automation using Selenium</t>
+  </si>
+  <si>
+    <t>Hourly basis service</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Cypress</t>
+  </si>
+  <si>
+    <t>SuccessMessage</t>
+  </si>
+  <si>
+    <t>Service Listing Updated successfully</t>
+  </si>
+  <si>
+    <t>Service Listing Added successfully</t>
+  </si>
+  <si>
+    <t>Automation using Selenium has been deleted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -88,12 +203,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,7 +233,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -120,6 +241,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1365,7 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1418,4 +1545,342 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="21.58203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.9140625" customWidth="1"/>
+    <col min="5" max="5" width="17.9140625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="8" max="8" width="12.58203125" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="15.4140625" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8">
+        <v>44528</v>
+      </c>
+      <c r="I2" s="8">
+        <v>44893</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="25.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8">
+        <v>44528</v>
+      </c>
+      <c r="I2" s="8">
+        <v>44893</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More updates nov11 (#4)
* ProfileUpdates

* ProfileUpdates

* Code Refactoring and API Postman Collections
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Mars.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Mars.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="520" windowWidth="13120" windowHeight="3740" activeTab="1"/>
+    <workbookView xWindow="530" yWindow="520" windowWidth="13120" windowHeight="3740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="SignUp" sheetId="2" r:id="rId2"/>
+    <sheet name="AddSkill" sheetId="3" r:id="rId3"/>
+    <sheet name="UpdateSkill" sheetId="4" r:id="rId4"/>
+    <sheet name="RemoveSkill" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>username</t>
   </si>
@@ -54,12 +57,124 @@
   </si>
   <si>
     <t>Eer</t>
+  </si>
+  <si>
+    <t>Would like to provide selenium training for beginners</t>
+  </si>
+  <si>
+    <t>Programming &amp; Tech</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>One-off service</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Skill-Exchange</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>LocationType</t>
+  </si>
+  <si>
+    <t>Startdate</t>
+  </si>
+  <si>
+    <t>Enddate</t>
+  </si>
+  <si>
+    <t>Selectday</t>
+  </si>
+  <si>
+    <t>Starttime</t>
+  </si>
+  <si>
+    <t>Endtime</t>
+  </si>
+  <si>
+    <t>SkillTrade</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Selenium Web Driver</t>
+  </si>
+  <si>
+    <t>Keen to teach API testing using Postman tool</t>
+  </si>
+  <si>
+    <t>Automation using Selenium</t>
+  </si>
+  <si>
+    <t>Hourly basis service</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Cypress</t>
+  </si>
+  <si>
+    <t>SuccessMessage</t>
+  </si>
+  <si>
+    <t>Service Listing Updated successfully</t>
+  </si>
+  <si>
+    <t>Service Listing Added successfully</t>
+  </si>
+  <si>
+    <t>Automation using Selenium has been deleted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -88,12 +203,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,7 +233,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -120,6 +241,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1365,7 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1418,4 +1545,342 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="21.58203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.9140625" customWidth="1"/>
+    <col min="5" max="5" width="17.9140625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="8" max="8" width="12.58203125" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="15.4140625" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8">
+        <v>44528</v>
+      </c>
+      <c r="I2" s="8">
+        <v>44893</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="25.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8">
+        <v>44528</v>
+      </c>
+      <c r="I2" s="8">
+        <v>44893</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>